<commit_message>
Finished processing of dates and age models
</commit_message>
<xml_diff>
--- a/Timing_Sr_spikes.xlsx
+++ b/Timing_Sr_spikes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwi213\Dropbox\Research\Manuscripts\TE spike recognition and environmental factors (Sanne Christian)\Cleanalyze_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75F0F45D-BA69-45EA-93C2-B40E27B80418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64382A06-8B57-4AC5-AA53-FE0185220D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30048" yWindow="1272" windowWidth="21600" windowHeight="11292" xr2:uid="{C3CE8052-BAB1-484F-A492-E980C192A710}"/>
+    <workbookView xWindow="-29472" yWindow="1248" windowWidth="23040" windowHeight="12168" xr2:uid="{C3CE8052-BAB1-484F-A492-E980C192A710}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>Subtidal</t>
   </si>
@@ -74,27 +74,15 @@
     <t>11-05-202111:00</t>
   </si>
   <si>
-    <t>12-05-202111:00</t>
-  </si>
-  <si>
     <t>low</t>
   </si>
   <si>
-    <t>11-05-202112:00</t>
-  </si>
-  <si>
     <t>31-05-202115:00</t>
   </si>
   <si>
     <t>01-06-202115:00</t>
   </si>
   <si>
-    <t>27-06-202113:00</t>
-  </si>
-  <si>
-    <t>28-06-202113:00</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -110,10 +98,43 @@
     <t>12-08-202114:00</t>
   </si>
   <si>
-    <t>08-09-202114:00</t>
-  </si>
-  <si>
     <t>09-09-202114:00</t>
+  </si>
+  <si>
+    <t>11-05-202110:40</t>
+  </si>
+  <si>
+    <t>12-05-202110:50</t>
+  </si>
+  <si>
+    <t>12-05-202111:10</t>
+  </si>
+  <si>
+    <t>31-05-202115:30</t>
+  </si>
+  <si>
+    <t>01-06-202115:30</t>
+  </si>
+  <si>
+    <t>27-06-202113:30</t>
+  </si>
+  <si>
+    <t>28-06-202112:45</t>
+  </si>
+  <si>
+    <t>28-06-202113:15</t>
+  </si>
+  <si>
+    <t>12-08-202113:40</t>
+  </si>
+  <si>
+    <t>11-08-202113:40</t>
+  </si>
+  <si>
+    <t>08-09-202113:20</t>
+  </si>
+  <si>
+    <t>08-09-202113:40</t>
   </si>
 </sst>
 </file>
@@ -488,7 +509,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,13 +562,13 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -558,13 +579,13 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -575,10 +596,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -592,10 +613,10 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -609,13 +630,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,13 +647,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -643,10 +664,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -660,10 +681,10 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -677,13 +698,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,13 +715,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,10 +732,10 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -728,10 +749,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>

</xml_diff>